<commit_message>
Fixed Mouser PN for 22uF caps
</commit_message>
<xml_diff>
--- a/BOM/Magpie Plancks (frames).xlsx
+++ b/BOM/Magpie Plancks (frames).xlsx
@@ -106,7 +106,7 @@
     <t xml:space="preserve">CPOL-USC</t>
   </si>
   <si>
-    <t xml:space="preserve">667-HA1C220WR</t>
+    <t xml:space="preserve">667-EEE-HA1C220WR</t>
   </si>
   <si>
     <t xml:space="preserve">R6, R7, R8, R9,  R16, R19, R20, R21, R22</t>
@@ -670,7 +670,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>